<commit_message>
More conf.matrices and plots, improved histogram
</commit_message>
<xml_diff>
--- a/Plots/confmatrix_NN.xlsx
+++ b/Plots/confmatrix_NN.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inge\Documents\GitHub\TTT4275_Classification_Project\Plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBB6596-4903-4EE7-B172-101160085BF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7898ADA-2083-44B8-8693-FC154667FBAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5BB9F2A5-5F85-4EBE-9F0E-DF94768C017C}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{5BB9F2A5-5F85-4EBE-9F0E-DF94768C017C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="IRIS" sheetId="2" r:id="rId1"/>
+    <sheet name="NMIST" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>ER:  0.0369</t>
   </si>
@@ -70,6 +71,84 @@
   </si>
   <si>
     <t>Clustering k=1</t>
+  </si>
+  <si>
+    <t>0.]</t>
+  </si>
+  <si>
+    <t>1.]</t>
+  </si>
+  <si>
+    <t>Training set error rate:  0.0333</t>
+  </si>
+  <si>
+    <t>Verification set error rate:  0.0333</t>
+  </si>
+  <si>
+    <t>ts first 30</t>
+  </si>
+  <si>
+    <t>vs 20 last</t>
+  </si>
+  <si>
+    <t>ts last 30</t>
+  </si>
+  <si>
+    <t>2.]</t>
+  </si>
+  <si>
+    <t>vs: 20 first</t>
+  </si>
+  <si>
+    <t>Training set error rate:  0.0555</t>
+  </si>
+  <si>
+    <t>Verification set error rate:  0.0166</t>
+  </si>
+  <si>
+    <t>ts fist30, vs last20</t>
+  </si>
+  <si>
+    <t>Removed feature 1</t>
+  </si>
+  <si>
+    <t>[30.</t>
+  </si>
+  <si>
+    <t>29.]</t>
+  </si>
+  <si>
+    <t>Verification set error rate:  0.05</t>
+  </si>
+  <si>
+    <t>Removed feature 0</t>
+  </si>
+  <si>
+    <t>28.]</t>
+  </si>
+  <si>
+    <t>Training set error rate:  0.111</t>
+  </si>
+  <si>
+    <t>[20.</t>
+  </si>
+  <si>
+    <t>18.]</t>
+  </si>
+  <si>
+    <t>Verification set error rate:  0.0833</t>
+  </si>
+  <si>
+    <t>Removed feature 3</t>
+  </si>
+  <si>
+    <t>Training set error rate:  0.177</t>
+  </si>
+  <si>
+    <t>20.]</t>
+  </si>
+  <si>
+    <t>Verification set error rate:  0.1</t>
   </si>
 </sst>
 </file>
@@ -239,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -317,6 +396,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -638,11 +723,492 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B817E63-2FB3-4FDB-83D9-1F8AF47F59F7}">
+  <dimension ref="A4:AE32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="5" width="3.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="S4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="22">
+        <v>0</v>
+      </c>
+      <c r="D6" s="22">
+        <v>1</v>
+      </c>
+      <c r="E6" s="23">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="N6" s="18">
+        <v>30</v>
+      </c>
+      <c r="O6" s="18">
+        <v>0</v>
+      </c>
+      <c r="P6" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18">
+        <v>20</v>
+      </c>
+      <c r="U6" s="18">
+        <v>0</v>
+      </c>
+      <c r="V6" s="18">
+        <v>0</v>
+      </c>
+      <c r="W6" s="18"/>
+    </row>
+    <row r="7" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="20">
+        <v>0</v>
+      </c>
+      <c r="C7" s="30">
+        <v>30</v>
+      </c>
+      <c r="D7" s="30">
+        <v>0</v>
+      </c>
+      <c r="E7" s="29">
+        <v>0</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="18">
+        <v>20</v>
+      </c>
+      <c r="I7" s="18">
+        <v>0</v>
+      </c>
+      <c r="J7" s="19">
+        <v>0</v>
+      </c>
+      <c r="K7" s="19"/>
+      <c r="N7" s="18">
+        <v>0</v>
+      </c>
+      <c r="O7" s="18">
+        <v>27</v>
+      </c>
+      <c r="P7" s="18">
+        <v>2</v>
+      </c>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18">
+        <v>0</v>
+      </c>
+      <c r="U7" s="18">
+        <v>19</v>
+      </c>
+      <c r="V7" s="18">
+        <v>0</v>
+      </c>
+      <c r="X7" s="18"/>
+      <c r="AD7" s="18"/>
+      <c r="AE7" s="18"/>
+    </row>
+    <row r="8" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="20">
+        <v>1</v>
+      </c>
+      <c r="C8" s="30">
+        <v>0</v>
+      </c>
+      <c r="D8" s="30">
+        <v>28</v>
+      </c>
+      <c r="E8" s="25">
+        <v>1</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19">
+        <v>0</v>
+      </c>
+      <c r="I8" s="19">
+        <v>18</v>
+      </c>
+      <c r="J8" s="19">
+        <v>0</v>
+      </c>
+      <c r="K8" s="18"/>
+      <c r="N8" s="18">
+        <v>0</v>
+      </c>
+      <c r="O8" s="18">
+        <v>3</v>
+      </c>
+      <c r="P8" s="18">
+        <v>28</v>
+      </c>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18">
+        <v>0</v>
+      </c>
+      <c r="U8" s="18">
+        <v>1</v>
+      </c>
+      <c r="V8" s="18">
+        <v>20</v>
+      </c>
+      <c r="X8" s="18"/>
+      <c r="AE8" s="18"/>
+    </row>
+    <row r="9" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="21">
+        <v>2</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0</v>
+      </c>
+      <c r="D9" s="27">
+        <v>2</v>
+      </c>
+      <c r="E9" s="28">
+        <v>29</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19">
+        <v>0</v>
+      </c>
+      <c r="I9" s="19">
+        <v>2</v>
+      </c>
+      <c r="J9" s="19">
+        <v>20</v>
+      </c>
+      <c r="K9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="AE9" s="18"/>
+    </row>
+    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="N10" t="s">
+        <v>21</v>
+      </c>
+      <c r="T10" t="s">
+        <v>22</v>
+      </c>
+      <c r="X10" s="18"/>
+      <c r="AD10" s="18"/>
+      <c r="AE10" s="18"/>
+    </row>
+    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20">
+        <v>30</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>28</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>22</v>
+      </c>
+      <c r="J21" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>14</v>
+      </c>
+      <c r="N21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>8</v>
+      </c>
+      <c r="J22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>16</v>
+      </c>
+      <c r="N22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L28" t="s">
+        <v>31</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>18</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>17</v>
+      </c>
+      <c r="J29" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>14</v>
+      </c>
+      <c r="N29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>19</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="J30" t="s">
+        <v>32</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>5</v>
+      </c>
+      <c r="N30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" t="s">
+        <v>33</v>
+      </c>
+      <c r="L32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C7:E9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="3"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C54487B-A889-4956-9D31-E92E5D209DE3}">
   <dimension ref="E2:AX60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="101" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z28" sqref="Z28"/>
+    <sheetView topLeftCell="C1" zoomScale="101" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +1220,8 @@
     <col min="18" max="18" width="4" customWidth="1"/>
     <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="28" width="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="28" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="5:50" x14ac:dyDescent="0.25">
@@ -2117,129 +2684,94 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="R24" s="1"/>
-      <c r="T24" s="1"/>
-    </row>
-    <row r="25" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="R25" s="1"/>
-      <c r="T25" s="1"/>
-    </row>
-    <row r="26" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="R26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-    </row>
-    <row r="27" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="R27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-    </row>
-    <row r="28" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="R28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-    </row>
-    <row r="29" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="R29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-    </row>
-    <row r="30" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-    </row>
-    <row r="31" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-    </row>
     <row r="32" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="R32" s="1"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
     </row>
-    <row r="33" spans="17:22" x14ac:dyDescent="0.25">
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-    </row>
-    <row r="34" spans="17:22" x14ac:dyDescent="0.25">
-      <c r="R34" s="1"/>
+    <row r="33" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+    </row>
+    <row r="34" spans="16:22" x14ac:dyDescent="0.25">
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
     </row>
-    <row r="35" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="16:22" x14ac:dyDescent="0.25">
       <c r="R35" s="1"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
     </row>
-    <row r="36" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="16:22" x14ac:dyDescent="0.25">
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="16:22" x14ac:dyDescent="0.25">
       <c r="R37" s="1"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
     </row>
-    <row r="38" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="16:22" x14ac:dyDescent="0.25">
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="16:22" x14ac:dyDescent="0.25">
       <c r="R39" s="1"/>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
     </row>
-    <row r="40" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="16:22" x14ac:dyDescent="0.25">
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
     </row>
-    <row r="41" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="16:22" x14ac:dyDescent="0.25">
       <c r="R41" s="1"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
     </row>
-    <row r="42" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="16:22" x14ac:dyDescent="0.25">
       <c r="R42" s="1"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
     </row>
-    <row r="43" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="16:22" x14ac:dyDescent="0.25">
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
     </row>
-    <row r="44" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="16:22" x14ac:dyDescent="0.25">
       <c r="R44" s="1"/>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
     </row>
-    <row r="45" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="16:22" x14ac:dyDescent="0.25">
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="16:22" x14ac:dyDescent="0.25">
       <c r="R46" s="1"/>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
     </row>
-    <row r="47" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="16:22" x14ac:dyDescent="0.25">
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="17:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="16:22" x14ac:dyDescent="0.25">
       <c r="R48" s="1"/>
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>

</xml_diff>

<commit_message>
Finished report and more testing in code
</commit_message>
<xml_diff>
--- a/Plots/confmatrix_NN.xlsx
+++ b/Plots/confmatrix_NN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inge\Documents\GitHub\TTT4275_Classification_Project\Plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7898ADA-2083-44B8-8693-FC154667FBAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75601BB2-E740-453E-BC76-F1919B7DB213}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{5BB9F2A5-5F85-4EBE-9F0E-DF94768C017C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5BB9F2A5-5F85-4EBE-9F0E-DF94768C017C}"/>
   </bookViews>
   <sheets>
     <sheet name="IRIS" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>ER:  0.0369</t>
   </si>
@@ -73,82 +73,82 @@
     <t>Clustering k=1</t>
   </si>
   <si>
-    <t>0.]</t>
-  </si>
-  <si>
-    <t>1.]</t>
-  </si>
-  <si>
-    <t>Training set error rate:  0.0333</t>
-  </si>
-  <si>
-    <t>Verification set error rate:  0.0333</t>
-  </si>
-  <si>
-    <t>ts first 30</t>
-  </si>
-  <si>
-    <t>vs 20 last</t>
-  </si>
-  <si>
-    <t>ts last 30</t>
-  </si>
-  <si>
-    <t>2.]</t>
-  </si>
-  <si>
-    <t>vs: 20 first</t>
-  </si>
-  <si>
-    <t>Training set error rate:  0.0555</t>
-  </si>
-  <si>
-    <t>Verification set error rate:  0.0166</t>
-  </si>
-  <si>
     <t>ts fist30, vs last20</t>
   </si>
   <si>
     <t>Removed feature 1</t>
   </si>
   <si>
-    <t>[30.</t>
-  </si>
-  <si>
-    <t>29.]</t>
-  </si>
-  <si>
-    <t>Verification set error rate:  0.05</t>
-  </si>
-  <si>
-    <t>Removed feature 0</t>
-  </si>
-  <si>
-    <t>28.]</t>
-  </si>
-  <si>
-    <t>Training set error rate:  0.111</t>
-  </si>
-  <si>
-    <t>[20.</t>
-  </si>
-  <si>
-    <t>18.]</t>
-  </si>
-  <si>
-    <t>Verification set error rate:  0.0833</t>
-  </si>
-  <si>
-    <t>Removed feature 3</t>
-  </si>
-  <si>
-    <t>Training set error rate:  0.177</t>
-  </si>
-  <si>
-    <t>20.]</t>
-  </si>
-  <si>
-    <t>Verification set error rate:  0.1</t>
+    <t>ts ER =  3.33%</t>
+  </si>
+  <si>
+    <t>Removed feature 1 &amp; 0</t>
+  </si>
+  <si>
+    <t>ts ER = 11.1%</t>
+  </si>
+  <si>
+    <t>vs ER = 5%</t>
+  </si>
+  <si>
+    <t>vs ER = 8.33%</t>
+  </si>
+  <si>
+    <t>ts ER = 12.2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Removed feature 1, 0 &amp; 2 </t>
+  </si>
+  <si>
+    <t>Only feature 0</t>
+  </si>
+  <si>
+    <t>Only feature 1</t>
+  </si>
+  <si>
+    <t>ts ER =  17.7%</t>
+  </si>
+  <si>
+    <t>vs ER = 10%</t>
+  </si>
+  <si>
+    <t>ts ER = 37.7%</t>
+  </si>
+  <si>
+    <t>ts ER 45.5%</t>
+  </si>
+  <si>
+    <t>vs ER 33.3%</t>
+  </si>
+  <si>
+    <t>vs ER 41.6%</t>
+  </si>
+  <si>
+    <t>ts ER = 3.33%</t>
+  </si>
+  <si>
+    <t>vs ER = 3.33%</t>
+  </si>
+  <si>
+    <t>ts ER = 5.56%</t>
+  </si>
+  <si>
+    <t>vs ER = 1.67%</t>
+  </si>
+  <si>
+    <t>First 30 samples</t>
+  </si>
+  <si>
+    <t>Last 20 samples</t>
+  </si>
+  <si>
+    <t>Last 30 samples</t>
+  </si>
+  <si>
+    <t>First 20 samples</t>
+  </si>
+  <si>
+    <t>Only feature 2</t>
   </si>
 </sst>
 </file>
@@ -318,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -403,6 +403,17 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -724,475 +735,1174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B817E63-2FB3-4FDB-83D9-1F8AF47F59F7}">
-  <dimension ref="A4:AE32"/>
+  <dimension ref="A2:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AD22" sqref="AD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="3.5703125" customWidth="1"/>
+    <col min="2" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="10" width="4.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="12" max="15" width="4" customWidth="1"/>
+    <col min="16" max="16" width="10" customWidth="1"/>
+    <col min="17" max="20" width="4" customWidth="1"/>
+    <col min="23" max="28" width="4.140625" customWidth="1"/>
+    <col min="29" max="29" width="4" customWidth="1"/>
+    <col min="31" max="34" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="22">
+        <v>0</v>
+      </c>
+      <c r="D3" s="22">
+        <v>1</v>
+      </c>
+      <c r="E3" s="23">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="22">
+        <v>0</v>
+      </c>
+      <c r="I3" s="22">
+        <v>1</v>
+      </c>
+      <c r="J3" s="23">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="20">
+        <v>0</v>
+      </c>
+      <c r="C4" s="30">
+        <v>30</v>
+      </c>
+      <c r="D4" s="30">
+        <v>0</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20">
+        <v>0</v>
+      </c>
+      <c r="H4" s="31">
+        <v>20</v>
+      </c>
+      <c r="I4" s="31">
+        <v>0</v>
+      </c>
+      <c r="J4" s="25">
+        <v>0</v>
+      </c>
+      <c r="K4" s="19"/>
+      <c r="U4" s="18"/>
+    </row>
+    <row r="5" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="20">
+        <v>1</v>
+      </c>
+      <c r="C5" s="30">
+        <v>0</v>
+      </c>
+      <c r="D5" s="30">
+        <v>28</v>
+      </c>
+      <c r="E5" s="25">
+        <v>1</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20">
+        <v>1</v>
+      </c>
+      <c r="H5" s="30">
+        <v>0</v>
+      </c>
+      <c r="I5" s="30">
+        <v>18</v>
+      </c>
+      <c r="J5" s="25">
+        <v>0</v>
+      </c>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="21">
+        <v>2</v>
+      </c>
+      <c r="C6" s="26">
+        <v>0</v>
+      </c>
+      <c r="D6" s="27">
+        <v>2</v>
+      </c>
+      <c r="E6" s="28">
+        <v>29</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="21">
+        <v>2</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0</v>
+      </c>
+      <c r="I6" s="27">
+        <v>2</v>
+      </c>
+      <c r="J6" s="28">
+        <v>20</v>
+      </c>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="U7" s="18"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="18"/>
+    </row>
+    <row r="8" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V8" s="18"/>
+      <c r="AC8" s="18"/>
+    </row>
+    <row r="9" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="V9" s="18"/>
+      <c r="AC9" s="18"/>
+    </row>
+    <row r="10" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="22">
+        <v>0</v>
+      </c>
+      <c r="D10" s="22">
+        <v>1</v>
+      </c>
+      <c r="E10" s="23">
+        <v>2</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="22">
+        <v>0</v>
+      </c>
+      <c r="I10" s="22">
+        <v>1</v>
+      </c>
+      <c r="J10" s="23">
+        <v>2</v>
+      </c>
+      <c r="V10" s="18"/>
+      <c r="AB10" s="18"/>
+      <c r="AC10" s="18"/>
+    </row>
+    <row r="11" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="20">
+        <v>0</v>
+      </c>
+      <c r="C11" s="31">
+        <v>30</v>
+      </c>
+      <c r="D11" s="31">
+        <v>0</v>
+      </c>
+      <c r="E11" s="32">
+        <v>0</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="20">
+        <v>0</v>
+      </c>
+      <c r="H11" s="31">
+        <v>20</v>
+      </c>
+      <c r="I11" s="31">
+        <v>0</v>
+      </c>
+      <c r="J11" s="32">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="V11" s="18"/>
+    </row>
+    <row r="12" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="20">
+        <v>1</v>
+      </c>
+      <c r="C12" s="31">
+        <v>0</v>
+      </c>
+      <c r="D12" s="31">
+        <v>27</v>
+      </c>
+      <c r="E12" s="32">
+        <v>2</v>
+      </c>
+      <c r="G12" s="20">
+        <v>1</v>
+      </c>
+      <c r="H12" s="31">
+        <v>0</v>
+      </c>
+      <c r="I12" s="31">
+        <v>19</v>
+      </c>
+      <c r="J12" s="32">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="21">
+        <v>2</v>
+      </c>
+      <c r="C13" s="33">
+        <v>0</v>
+      </c>
+      <c r="D13" s="33">
+        <v>3</v>
+      </c>
+      <c r="E13" s="34">
+        <v>28</v>
+      </c>
+      <c r="G13" s="21">
+        <v>2</v>
+      </c>
+      <c r="H13" s="33">
+        <v>0</v>
+      </c>
+      <c r="I13" s="33">
+        <v>1</v>
+      </c>
+      <c r="J13" s="34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="Q18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="22">
+        <v>0</v>
+      </c>
+      <c r="D19" s="22">
+        <v>1</v>
+      </c>
+      <c r="E19" s="23">
+        <v>2</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="22">
+        <v>0</v>
+      </c>
+      <c r="I19" s="22">
+        <v>1</v>
+      </c>
+      <c r="J19" s="23">
+        <v>2</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" s="22">
+        <v>0</v>
+      </c>
+      <c r="N19" s="22">
+        <v>1</v>
+      </c>
+      <c r="O19" s="23">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R19" s="22">
+        <v>0</v>
+      </c>
+      <c r="S19" s="22">
+        <v>1</v>
+      </c>
+      <c r="T19" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="35">
+        <v>30</v>
+      </c>
+      <c r="D20" s="35">
+        <v>0</v>
+      </c>
+      <c r="E20" s="36">
+        <v>0</v>
+      </c>
+      <c r="G20" s="20">
+        <v>0</v>
+      </c>
+      <c r="H20" s="35">
+        <v>20</v>
+      </c>
+      <c r="I20" s="35">
+        <v>0</v>
+      </c>
+      <c r="J20" s="36">
+        <v>0</v>
+      </c>
+      <c r="L20" s="20">
+        <v>0</v>
+      </c>
+      <c r="M20" s="35">
+        <v>30</v>
+      </c>
+      <c r="N20" s="35">
+        <v>0</v>
+      </c>
+      <c r="O20" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="20">
+        <v>0</v>
+      </c>
+      <c r="R20" s="35">
+        <v>20</v>
+      </c>
+      <c r="S20" s="35">
+        <v>0</v>
+      </c>
+      <c r="T20" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="20">
+        <v>1</v>
+      </c>
+      <c r="C21" s="35">
+        <v>0</v>
+      </c>
+      <c r="D21" s="35">
+        <v>28</v>
+      </c>
+      <c r="E21" s="36">
+        <v>1</v>
+      </c>
+      <c r="G21" s="20">
+        <v>1</v>
+      </c>
+      <c r="H21" s="35">
+        <v>0</v>
+      </c>
+      <c r="I21" s="35">
+        <v>18</v>
+      </c>
+      <c r="J21" s="36">
+        <v>1</v>
+      </c>
+      <c r="L21" s="20">
+        <v>1</v>
+      </c>
+      <c r="M21" s="35">
+        <v>0</v>
+      </c>
+      <c r="N21" s="35">
+        <v>22</v>
+      </c>
+      <c r="O21" s="36">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="20">
+        <v>1</v>
+      </c>
+      <c r="R21" s="35">
+        <v>0</v>
+      </c>
+      <c r="S21" s="35">
         <v>17</v>
       </c>
-      <c r="N4" t="s">
+      <c r="T21" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="21">
+        <v>2</v>
+      </c>
+      <c r="C22" s="37">
+        <v>0</v>
+      </c>
+      <c r="D22" s="37">
+        <v>2</v>
+      </c>
+      <c r="E22" s="38">
+        <v>29</v>
+      </c>
+      <c r="G22" s="21">
+        <v>2</v>
+      </c>
+      <c r="H22" s="37">
+        <v>0</v>
+      </c>
+      <c r="I22" s="37">
+        <v>2</v>
+      </c>
+      <c r="J22" s="38">
+        <v>19</v>
+      </c>
+      <c r="L22" s="21">
+        <v>2</v>
+      </c>
+      <c r="M22" s="37">
+        <v>0</v>
+      </c>
+      <c r="N22" s="37">
+        <v>8</v>
+      </c>
+      <c r="O22" s="38">
+        <v>28</v>
+      </c>
+      <c r="Q22" s="21">
+        <v>2</v>
+      </c>
+      <c r="R22" s="37">
+        <v>0</v>
+      </c>
+      <c r="S22" s="37">
+        <v>3</v>
+      </c>
+      <c r="T22" s="38">
         <v>18</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="S4" t="s">
+    </row>
+    <row r="23" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+      <c r="L25" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="22">
+        <v>0</v>
+      </c>
+      <c r="D26" s="22">
+        <v>1</v>
+      </c>
+      <c r="E26" s="23">
+        <v>2</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="22">
+        <v>0</v>
+      </c>
+      <c r="I26" s="22">
+        <v>1</v>
+      </c>
+      <c r="J26" s="23">
+        <v>2</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M26" s="22">
+        <v>0</v>
+      </c>
+      <c r="N26" s="22">
+        <v>1</v>
+      </c>
+      <c r="O26" s="23">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R26" s="22">
+        <v>0</v>
+      </c>
+      <c r="S26" s="22">
+        <v>1</v>
+      </c>
+      <c r="T26" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="20">
+        <v>0</v>
+      </c>
+      <c r="C27" s="35">
+        <v>30</v>
+      </c>
+      <c r="D27" s="35">
+        <v>0</v>
+      </c>
+      <c r="E27" s="36">
+        <v>0</v>
+      </c>
+      <c r="G27" s="20">
+        <v>0</v>
+      </c>
+      <c r="H27" s="35">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="22">
-        <v>0</v>
-      </c>
-      <c r="D6" s="22">
-        <v>1</v>
-      </c>
-      <c r="E6" s="23">
-        <v>2</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="N6" s="18">
+      <c r="I27" s="35">
+        <v>0</v>
+      </c>
+      <c r="J27" s="36">
+        <v>0</v>
+      </c>
+      <c r="L27" s="20">
+        <v>0</v>
+      </c>
+      <c r="M27" s="35">
         <v>30</v>
       </c>
-      <c r="O6" s="18">
-        <v>0</v>
-      </c>
-      <c r="P6" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18">
+      <c r="N27" s="35">
+        <v>0</v>
+      </c>
+      <c r="O27" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="20">
+        <v>0</v>
+      </c>
+      <c r="R27" s="35">
         <v>20</v>
       </c>
-      <c r="U6" s="18">
-        <v>0</v>
-      </c>
-      <c r="V6" s="18">
-        <v>0</v>
-      </c>
-      <c r="W6" s="18"/>
-    </row>
-    <row r="7" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="20">
-        <v>0</v>
-      </c>
-      <c r="C7" s="30">
+      <c r="S27" s="35">
+        <v>1</v>
+      </c>
+      <c r="T27" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="20">
+        <v>1</v>
+      </c>
+      <c r="C28" s="35">
+        <v>0</v>
+      </c>
+      <c r="D28" s="35">
+        <v>19</v>
+      </c>
+      <c r="E28" s="36">
+        <v>0</v>
+      </c>
+      <c r="G28" s="20">
+        <v>1</v>
+      </c>
+      <c r="H28" s="35">
+        <v>0</v>
+      </c>
+      <c r="I28" s="35">
+        <v>16</v>
+      </c>
+      <c r="J28" s="36">
+        <v>1</v>
+      </c>
+      <c r="L28" s="20">
+        <v>1</v>
+      </c>
+      <c r="M28" s="35">
+        <v>0</v>
+      </c>
+      <c r="N28" s="35">
+        <v>14</v>
+      </c>
+      <c r="O28" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="20">
+        <v>1</v>
+      </c>
+      <c r="R28" s="35">
+        <v>0</v>
+      </c>
+      <c r="S28" s="35">
+        <v>14</v>
+      </c>
+      <c r="T28" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="21">
+        <v>2</v>
+      </c>
+      <c r="C29" s="37">
+        <v>0</v>
+      </c>
+      <c r="D29" s="37">
+        <v>11</v>
+      </c>
+      <c r="E29" s="38">
         <v>30</v>
       </c>
-      <c r="D7" s="30">
-        <v>0</v>
-      </c>
-      <c r="E7" s="29">
-        <v>0</v>
-      </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="18">
+      <c r="G29" s="21">
+        <v>2</v>
+      </c>
+      <c r="H29" s="37">
+        <v>0</v>
+      </c>
+      <c r="I29" s="37">
+        <v>4</v>
+      </c>
+      <c r="J29" s="38">
+        <v>19</v>
+      </c>
+      <c r="L29" s="21">
+        <v>2</v>
+      </c>
+      <c r="M29" s="37">
+        <v>0</v>
+      </c>
+      <c r="N29" s="37">
+        <v>16</v>
+      </c>
+      <c r="O29" s="38">
+        <v>30</v>
+      </c>
+      <c r="Q29" s="21">
+        <v>2</v>
+      </c>
+      <c r="R29" s="37">
+        <v>0</v>
+      </c>
+      <c r="S29" s="37">
+        <v>5</v>
+      </c>
+      <c r="T29" s="38">
         <v>20</v>
       </c>
-      <c r="I7" s="18">
-        <v>0</v>
-      </c>
-      <c r="J7" s="19">
-        <v>0</v>
-      </c>
-      <c r="K7" s="19"/>
-      <c r="N7" s="18">
-        <v>0</v>
-      </c>
-      <c r="O7" s="18">
+    </row>
+    <row r="30" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" t="s">
+        <v>20</v>
+      </c>
+      <c r="L30" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" t="s">
         <v>27</v>
       </c>
-      <c r="P7" s="18">
-        <v>2</v>
-      </c>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18">
-        <v>0</v>
-      </c>
-      <c r="U7" s="18">
-        <v>19</v>
-      </c>
-      <c r="V7" s="18">
-        <v>0</v>
-      </c>
-      <c r="X7" s="18"/>
-      <c r="AD7" s="18"/>
-      <c r="AE7" s="18"/>
-    </row>
-    <row r="8" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="20">
-        <v>1</v>
-      </c>
-      <c r="C8" s="30">
-        <v>0</v>
-      </c>
-      <c r="D8" s="30">
+      <c r="L32" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q32" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="25">
-        <v>1</v>
-      </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19">
-        <v>0</v>
-      </c>
-      <c r="I8" s="19">
+    </row>
+    <row r="33" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="22">
+        <v>0</v>
+      </c>
+      <c r="D33" s="22">
+        <v>1</v>
+      </c>
+      <c r="E33" s="23">
+        <v>2</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H33" s="22">
+        <v>0</v>
+      </c>
+      <c r="I33" s="22">
+        <v>1</v>
+      </c>
+      <c r="J33" s="23">
+        <v>2</v>
+      </c>
+      <c r="L33" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M33" s="22">
+        <v>0</v>
+      </c>
+      <c r="N33" s="22">
+        <v>1</v>
+      </c>
+      <c r="O33" s="23">
+        <v>2</v>
+      </c>
+      <c r="Q33" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R33" s="22">
+        <v>0</v>
+      </c>
+      <c r="S33" s="22">
+        <v>1</v>
+      </c>
+      <c r="T33" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="20">
+        <v>0</v>
+      </c>
+      <c r="C34" s="35">
+        <v>29</v>
+      </c>
+      <c r="D34" s="35">
+        <v>9</v>
+      </c>
+      <c r="E34" s="36">
+        <v>3</v>
+      </c>
+      <c r="G34" s="20">
+        <v>0</v>
+      </c>
+      <c r="H34" s="35">
+        <v>20</v>
+      </c>
+      <c r="I34" s="35">
+        <v>12</v>
+      </c>
+      <c r="J34" s="36">
+        <v>0</v>
+      </c>
+      <c r="L34" s="20">
+        <v>0</v>
+      </c>
+      <c r="M34" s="35">
+        <v>25</v>
+      </c>
+      <c r="N34" s="35">
+        <v>6</v>
+      </c>
+      <c r="O34" s="36">
+        <v>8</v>
+      </c>
+      <c r="Q34" s="20">
+        <v>0</v>
+      </c>
+      <c r="R34" s="35">
+        <v>17</v>
+      </c>
+      <c r="S34" s="35">
+        <v>2</v>
+      </c>
+      <c r="T34" s="36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="20">
+        <v>1</v>
+      </c>
+      <c r="C35" s="35">
+        <v>0</v>
+      </c>
+      <c r="D35" s="35">
+        <v>0</v>
+      </c>
+      <c r="E35" s="36">
+        <v>0</v>
+      </c>
+      <c r="G35" s="20">
+        <v>1</v>
+      </c>
+      <c r="H35" s="35">
+        <v>0</v>
+      </c>
+      <c r="I35" s="35">
+        <v>0</v>
+      </c>
+      <c r="J35" s="36">
+        <v>0</v>
+      </c>
+      <c r="L35" s="20">
+        <v>1</v>
+      </c>
+      <c r="M35" s="35">
+        <v>5</v>
+      </c>
+      <c r="N35" s="35">
+        <v>24</v>
+      </c>
+      <c r="O35" s="36">
+        <v>33</v>
+      </c>
+      <c r="Q35" s="20">
+        <v>1</v>
+      </c>
+      <c r="R35" s="35">
+        <v>3</v>
+      </c>
+      <c r="S35" s="35">
         <v>18</v>
       </c>
-      <c r="J8" s="19">
-        <v>0</v>
-      </c>
-      <c r="K8" s="18"/>
-      <c r="N8" s="18">
-        <v>0</v>
-      </c>
-      <c r="O8" s="18">
-        <v>3</v>
-      </c>
-      <c r="P8" s="18">
-        <v>28</v>
-      </c>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18">
-        <v>0</v>
-      </c>
-      <c r="U8" s="18">
-        <v>1</v>
-      </c>
-      <c r="V8" s="18">
+      <c r="T35" s="36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="21">
+        <v>2</v>
+      </c>
+      <c r="C36" s="37">
+        <v>1</v>
+      </c>
+      <c r="D36" s="37">
+        <v>21</v>
+      </c>
+      <c r="E36" s="38">
+        <v>27</v>
+      </c>
+      <c r="G36" s="21">
+        <v>2</v>
+      </c>
+      <c r="H36" s="37">
+        <v>0</v>
+      </c>
+      <c r="I36" s="37">
+        <v>8</v>
+      </c>
+      <c r="J36" s="38">
         <v>20</v>
       </c>
-      <c r="X8" s="18"/>
-      <c r="AE8" s="18"/>
-    </row>
-    <row r="9" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="21">
-        <v>2</v>
-      </c>
-      <c r="C9" s="26">
-        <v>0</v>
-      </c>
-      <c r="D9" s="27">
-        <v>2</v>
-      </c>
-      <c r="E9" s="28">
-        <v>29</v>
-      </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19">
-        <v>0</v>
-      </c>
-      <c r="I9" s="19">
-        <v>2</v>
-      </c>
-      <c r="J9" s="19">
-        <v>20</v>
-      </c>
-      <c r="K9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="AE9" s="18"/>
-    </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="N10" t="s">
+      <c r="L36" s="21">
+        <v>2</v>
+      </c>
+      <c r="M36" s="37">
+        <v>0</v>
+      </c>
+      <c r="N36" s="37">
+        <v>0</v>
+      </c>
+      <c r="O36" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="21">
+        <v>2</v>
+      </c>
+      <c r="R36" s="37">
+        <v>0</v>
+      </c>
+      <c r="S36" s="37">
+        <v>0</v>
+      </c>
+      <c r="T36" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>21</v>
       </c>
-      <c r="T10" t="s">
+      <c r="G37" t="s">
+        <v>21</v>
+      </c>
+      <c r="L37" t="s">
         <v>22</v>
       </c>
-      <c r="X10" s="18"/>
-      <c r="AD10" s="18"/>
-      <c r="AE10" s="18"/>
-    </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" t="s">
-        <v>28</v>
-      </c>
-      <c r="L18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
-        <v>12</v>
-      </c>
-      <c r="L20">
-        <v>30</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>28</v>
-      </c>
-      <c r="E21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
+      <c r="Q37" t="s">
         <v>22</v>
       </c>
-      <c r="J21" t="s">
-        <v>19</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>14</v>
-      </c>
-      <c r="N21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>8</v>
-      </c>
-      <c r="J22" t="s">
-        <v>29</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>16</v>
-      </c>
-      <c r="N22">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C28">
-        <v>20</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" t="s">
-        <v>31</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28" t="s">
-        <v>12</v>
-      </c>
-      <c r="L28" t="s">
-        <v>31</v>
-      </c>
-      <c r="M28">
-        <v>1</v>
-      </c>
-      <c r="N28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>18</v>
-      </c>
-      <c r="E29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>17</v>
-      </c>
-      <c r="J29" t="s">
-        <v>19</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>14</v>
-      </c>
-      <c r="N29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="E30">
-        <v>19</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>3</v>
-      </c>
-      <c r="J30" t="s">
-        <v>32</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <v>5</v>
-      </c>
-      <c r="N30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>27</v>
-      </c>
-      <c r="G32" t="s">
-        <v>33</v>
-      </c>
-      <c r="L32" t="s">
-        <v>37</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C7:E9">
+  <conditionalFormatting sqref="C4:E6">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="3"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:J6">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="3"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:E13">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="3"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="3"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="3"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11:J13">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="3"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:E22">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="3"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M20:O22">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="15"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M27:O29">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="25"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20:J22">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="3"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R20:T22">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="3"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R27:T29">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="3"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27:E29">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="25"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27:J29">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="7"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34:E36">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="25"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34:J36">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="20"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M34:O36">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="25"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R34:T36">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="15"/>
         <color theme="0"/>
         <color rgb="FFFF0000"/>
       </colorScale>

</xml_diff>